<commit_message>
fixed spreadsheet demo feedback issues (SHEET-241)
Add spacing between demo items
Use non-solid buttons in formatting demo
Remove extra space from upload demo
Update invoice example

Change-Id: I48012a59dc510049e782091ebfac6455323ea959
</commit_message>
<xml_diff>
--- a/src/main/resources/testsheets/Simple Invoice.xlsx
+++ b/src/main/resources/testsheets/Simple Invoice.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15620" yWindow="0" windowWidth="22540" windowHeight="22420" tabRatio="500"/>
+    <workbookView xWindow="15615" yWindow="0" windowWidth="22545" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
-  <si>
-    <t>Vaadin Spreadsheet Demo Ltd Invoice</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>547 Demo Suites #85</t>
   </si>
@@ -30,9 +27,6 @@
     <t>555-1234</t>
   </si>
   <si>
-    <t>vaadin.com</t>
-  </si>
-  <si>
     <t>Invoice No.</t>
   </si>
   <si>
@@ -75,12 +69,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Expert Services</t>
-  </si>
-  <si>
-    <t>Vaadin Spreadsheet License</t>
-  </si>
-  <si>
     <t>Subtotal</t>
   </si>
   <si>
@@ -91,6 +79,15 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Demo Ltd Invoice</t>
+  </si>
+  <si>
+    <t>Gardening Services</t>
+  </si>
+  <si>
+    <t>Ferns</t>
   </si>
 </sst>
 </file>
@@ -100,25 +97,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Open Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Open Sans"/>
     </font>
     <font>
       <u/>
@@ -136,16 +121,33 @@
     <font>
       <u/>
       <sz val="12"/>
-      <color theme="10"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Open Sans"/>
     </font>
     <font>
       <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Open Sans"/>
     </font>
   </fonts>
   <fills count="3">
@@ -200,34 +202,35 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -241,7 +244,42 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Open Sans"/>
         <scheme val="none"/>
@@ -259,7 +297,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Open Sans"/>
         <scheme val="none"/>
@@ -277,7 +315,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Open Sans"/>
         <scheme val="none"/>
@@ -294,7 +332,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Open Sans"/>
         <scheme val="none"/>
@@ -308,60 +346,30 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Open Sans"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Open Sans"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A14:D25" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A14:D25" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7">
   <autoFilter ref="A14:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Product" dataDxfId="3"/>
-    <tableColumn id="2" name="Units" dataDxfId="2"/>
-    <tableColumn id="3" name="Cost/Unit" dataDxfId="1"/>
-    <tableColumn id="4" name="Amount" dataDxfId="0">
+    <tableColumn id="1" name="Product" dataDxfId="5"/>
+    <tableColumn id="2" name="Units" dataDxfId="4"/>
+    <tableColumn id="3" name="Cost/Unit" dataDxfId="3"/>
+    <tableColumn id="4" name="Amount" dataDxfId="2">
       <calculatedColumnFormula>IF(B15,B15*C15,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -694,238 +702,264 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="17.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="18.33203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="37.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="1"/>
+    <col min="3" max="3" width="17.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="1"/>
+    <col min="6" max="6" width="18.375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="26.25">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="6"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75">
+      <c r="A14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="C9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="9" t="s">
+      <c r="C14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="A15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="5">
         <v>24</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="12">
         <v>150</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="12">
         <f>IF(B15,B15*C15,"")</f>
         <v>3600</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="5">
         <v>10</v>
       </c>
-      <c r="C16" s="8">
-        <v>690</v>
-      </c>
-      <c r="D16" s="8">
+      <c r="C16" s="12">
+        <v>50</v>
+      </c>
+      <c r="D16" s="12">
         <f t="shared" ref="D16:D24" si="0">IF(B16,B16*C16,"")</f>
-        <v>6900</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="C17" s="8"/>
-      <c r="D17" s="8" t="str">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="C18" s="8"/>
-      <c r="D18" s="8" t="str">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="C19" s="8"/>
-      <c r="D19" s="8" t="str">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="C20" s="8"/>
-      <c r="D20" s="8" t="str">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="C21" s="8"/>
-      <c r="D21" s="8" t="str">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="C22" s="8"/>
-      <c r="D22" s="8" t="str">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="C23" s="8"/>
-      <c r="D23" s="8" t="str">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="C24" s="8"/>
-      <c r="D24" s="8" t="str">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="C25" s="8"/>
-      <c r="D25" s="8" t="str">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12" t="str">
         <f>IF(B25,B25*C25,"")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="C26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="8">
+      <c r="C26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="12">
         <f>SUM(D15:D25)</f>
-        <v>10500</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="C27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="11">
+      <c r="C27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="13">
         <v>0.12</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="C28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="8">
+      <c r="C28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="12">
         <f>D26*D27</f>
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="14">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="15">
         <f>D26+D28</f>
-        <v>11760</v>
+        <v>4592</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="http://vaadin.com"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D26 D17 D18:D25" emptyCellReference="1"/>
   </ignoredErrors>

</xml_diff>